<commit_message>
Update script for Account and Lead
</commit_message>
<xml_diff>
--- a/src/test/resources/data/NewLeadTestData.xlsx
+++ b/src/test/resources/data/NewLeadTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ntpduong\Project\Selenium_Java\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06A9ED4-12FD-4831-87C0-A86BF8B5A5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296E7564-E472-4BDD-86C0-A68AF182C917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24690" yWindow="1260" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28002,9 +28002,9 @@
   </sheetPr>
   <dimension ref="A1:V701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A638" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>

</xml_diff>